<commit_message>
Completed easy part of merging changes from SWC
</commit_message>
<xml_diff>
--- a/tools/merge.xlsx
+++ b/tools/merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="175">
   <si>
     <t>bullet.cpp</t>
   </si>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>Merged</t>
+  </si>
+  <si>
+    <t>merged</t>
   </si>
   <si>
     <t>Percent</t>
@@ -991,7 +994,7 @@
   <dimension ref="A1:G165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1000,7 +1003,7 @@
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1039,7 +1042,7 @@
       </c>
       <c r="G2">
         <f>COUNTIFS(D2:D165,"merged")+COUNTIFS(D2:D165,"unneeded")</f>
-        <v>73</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1053,11 +1056,11 @@
         <v>167</v>
       </c>
       <c r="F3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G3">
         <f>G2*100/G1</f>
-        <v>44.512195121951223</v>
+        <v>70.731707317073173</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1076,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1086,6 +1089,9 @@
       <c r="C6" t="s">
         <v>167</v>
       </c>
+      <c r="D6" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
@@ -1094,6 +1100,9 @@
       <c r="C7" t="s">
         <v>167</v>
       </c>
+      <c r="D7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
@@ -1103,7 +1112,7 @@
         <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1114,7 +1123,7 @@
         <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1122,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1130,7 +1139,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1149,7 +1158,7 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1159,6 +1168,9 @@
       <c r="B14" t="s">
         <v>167</v>
       </c>
+      <c r="D14" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
@@ -1167,13 +1179,16 @@
       <c r="B15" t="s">
         <v>167</v>
       </c>
+      <c r="D15" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1181,7 +1196,7 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1200,7 +1215,7 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1208,7 +1223,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1218,6 +1233,9 @@
       <c r="C21" t="s">
         <v>167</v>
       </c>
+      <c r="D21" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
@@ -1235,7 +1253,7 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1256,13 +1274,16 @@
       <c r="C25" t="s">
         <v>167</v>
       </c>
+      <c r="D25" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1270,7 +1291,7 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1280,13 +1301,16 @@
       <c r="C28" t="s">
         <v>167</v>
       </c>
+      <c r="D28" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1307,6 +1331,9 @@
       <c r="B31" t="s">
         <v>167</v>
       </c>
+      <c r="D31" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
@@ -1326,6 +1353,9 @@
       <c r="B33" t="s">
         <v>167</v>
       </c>
+      <c r="D33" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
@@ -1356,6 +1386,9 @@
       <c r="C36" t="s">
         <v>167</v>
       </c>
+      <c r="D36" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
@@ -1364,6 +1397,9 @@
       <c r="C37" t="s">
         <v>167</v>
       </c>
+      <c r="D37" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
@@ -1383,6 +1419,9 @@
       <c r="B39" t="s">
         <v>167</v>
       </c>
+      <c r="D39" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
@@ -1400,7 +1439,7 @@
         <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1438,7 +1477,7 @@
         <v>43</v>
       </c>
       <c r="D45" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1457,7 +1496,7 @@
         <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1467,13 +1506,16 @@
       <c r="C48" t="s">
         <v>167</v>
       </c>
+      <c r="D48" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1483,13 +1525,16 @@
       <c r="C50" t="s">
         <v>167</v>
       </c>
+      <c r="D50" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1497,7 +1542,7 @@
         <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1508,7 +1553,7 @@
         <v>166</v>
       </c>
       <c r="D53" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1519,7 +1564,7 @@
         <v>166</v>
       </c>
       <c r="D54" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1530,7 +1575,7 @@
         <v>166</v>
       </c>
       <c r="D55" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1541,7 +1586,7 @@
         <v>166</v>
       </c>
       <c r="D56" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1551,13 +1596,16 @@
       <c r="C57" t="s">
         <v>167</v>
       </c>
+      <c r="D57" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1576,7 +1624,7 @@
         <v>58</v>
       </c>
       <c r="D60" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1595,7 +1643,7 @@
         <v>60</v>
       </c>
       <c r="D62" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1603,7 +1651,7 @@
         <v>61</v>
       </c>
       <c r="D63" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1611,7 +1659,7 @@
         <v>62</v>
       </c>
       <c r="D64" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1619,7 +1667,7 @@
         <v>63</v>
       </c>
       <c r="D65" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1627,7 +1675,7 @@
         <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1668,7 +1716,7 @@
         <v>68</v>
       </c>
       <c r="D70" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1676,7 +1724,7 @@
         <v>69</v>
       </c>
       <c r="D71" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1687,7 +1735,7 @@
         <v>166</v>
       </c>
       <c r="D72" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1698,7 +1746,7 @@
         <v>166</v>
       </c>
       <c r="D73" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1708,13 +1756,16 @@
       <c r="C74" t="s">
         <v>167</v>
       </c>
+      <c r="D74" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>73</v>
       </c>
       <c r="D75" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1768,6 +1819,9 @@
       <c r="B80" t="s">
         <v>167</v>
       </c>
+      <c r="D80" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
@@ -1776,6 +1830,9 @@
       <c r="B81" t="s">
         <v>167</v>
       </c>
+      <c r="D81" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
@@ -1784,6 +1841,9 @@
       <c r="B82" t="s">
         <v>167</v>
       </c>
+      <c r="D82" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
@@ -1792,6 +1852,9 @@
       <c r="B83" t="s">
         <v>167</v>
       </c>
+      <c r="D83" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
@@ -1800,13 +1863,16 @@
       <c r="B84" t="s">
         <v>167</v>
       </c>
+      <c r="D84" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>83</v>
       </c>
       <c r="D85" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1817,7 +1883,7 @@
         <v>166</v>
       </c>
       <c r="D86" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1849,6 +1915,9 @@
       <c r="C89" t="s">
         <v>167</v>
       </c>
+      <c r="D89" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
@@ -1857,6 +1926,9 @@
       <c r="B90" t="s">
         <v>166</v>
       </c>
+      <c r="D90" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
@@ -1865,6 +1937,9 @@
       <c r="B91" t="s">
         <v>166</v>
       </c>
+      <c r="D91" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
@@ -1881,6 +1956,9 @@
       <c r="A93" t="s">
         <v>91</v>
       </c>
+      <c r="D93" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
@@ -1897,6 +1975,9 @@
       <c r="A95" t="s">
         <v>93</v>
       </c>
+      <c r="D95" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
@@ -1938,6 +2019,9 @@
       <c r="B99" t="s">
         <v>167</v>
       </c>
+      <c r="D99" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
@@ -1974,7 +2058,7 @@
         <v>101</v>
       </c>
       <c r="D103" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1993,7 +2077,7 @@
         <v>103</v>
       </c>
       <c r="D105" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2003,6 +2087,9 @@
       <c r="C106" t="s">
         <v>167</v>
       </c>
+      <c r="D106" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
@@ -2011,6 +2098,9 @@
       <c r="B107" t="s">
         <v>167</v>
       </c>
+      <c r="D107" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
@@ -2028,7 +2118,7 @@
         <v>107</v>
       </c>
       <c r="D109" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2036,7 +2126,7 @@
         <v>108</v>
       </c>
       <c r="D110" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2044,7 +2134,7 @@
         <v>109</v>
       </c>
       <c r="D111" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2063,7 +2153,7 @@
         <v>111</v>
       </c>
       <c r="D113" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2084,6 +2174,9 @@
       <c r="B115" t="s">
         <v>167</v>
       </c>
+      <c r="D115" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
@@ -2092,6 +2185,9 @@
       <c r="B116" t="s">
         <v>167</v>
       </c>
+      <c r="D116" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
@@ -2100,6 +2196,9 @@
       <c r="B117" t="s">
         <v>167</v>
       </c>
+      <c r="D117" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
@@ -2108,13 +2207,16 @@
       <c r="C118" t="s">
         <v>167</v>
       </c>
+      <c r="D118" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>117</v>
       </c>
       <c r="D119" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2122,7 +2224,7 @@
         <v>118</v>
       </c>
       <c r="D120" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2130,7 +2232,7 @@
         <v>119</v>
       </c>
       <c r="D121" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2171,7 +2273,7 @@
         <v>123</v>
       </c>
       <c r="D125" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2181,6 +2283,9 @@
       <c r="B126" t="s">
         <v>167</v>
       </c>
+      <c r="D126" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
@@ -2189,13 +2294,16 @@
       <c r="C127" t="s">
         <v>167</v>
       </c>
+      <c r="D127" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>126</v>
       </c>
       <c r="D128" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2203,7 +2311,7 @@
         <v>127</v>
       </c>
       <c r="D129" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2213,6 +2321,9 @@
       <c r="C130" t="s">
         <v>167</v>
       </c>
+      <c r="D130" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
@@ -2221,13 +2332,16 @@
       <c r="C131" t="s">
         <v>167</v>
       </c>
+      <c r="D131" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>130</v>
       </c>
       <c r="D132" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2237,13 +2351,16 @@
       <c r="C133" t="s">
         <v>167</v>
       </c>
+      <c r="D133" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>132</v>
       </c>
       <c r="D134" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2284,7 +2401,7 @@
         <v>136</v>
       </c>
       <c r="D138" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2292,7 +2409,7 @@
         <v>137</v>
       </c>
       <c r="D139" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2300,7 +2417,7 @@
         <v>138</v>
       </c>
       <c r="D140" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2308,7 +2425,7 @@
         <v>139</v>
       </c>
       <c r="D141" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2316,7 +2433,7 @@
         <v>140</v>
       </c>
       <c r="D142" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2324,7 +2441,7 @@
         <v>141</v>
       </c>
       <c r="D143" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2332,7 +2449,7 @@
         <v>142</v>
       </c>
       <c r="D144" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2340,7 +2457,7 @@
         <v>143</v>
       </c>
       <c r="D145" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2348,7 +2465,7 @@
         <v>144</v>
       </c>
       <c r="D146" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2356,7 +2473,7 @@
         <v>145</v>
       </c>
       <c r="D147" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2364,7 +2481,7 @@
         <v>146</v>
       </c>
       <c r="D148" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2372,7 +2489,7 @@
         <v>147</v>
       </c>
       <c r="D149" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2380,7 +2497,7 @@
         <v>148</v>
       </c>
       <c r="D150" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2388,7 +2505,7 @@
         <v>149</v>
       </c>
       <c r="D151" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2396,7 +2513,7 @@
         <v>150</v>
       </c>
       <c r="D152" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2404,7 +2521,7 @@
         <v>151</v>
       </c>
       <c r="D153" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2412,7 +2529,7 @@
         <v>152</v>
       </c>
       <c r="D154" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2422,6 +2539,9 @@
       <c r="C155" t="s">
         <v>167</v>
       </c>
+      <c r="D155" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
@@ -2430,13 +2550,16 @@
       <c r="C156" t="s">
         <v>167</v>
       </c>
+      <c r="D156" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
         <v>155</v>
       </c>
       <c r="D157" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2444,7 +2567,7 @@
         <v>156</v>
       </c>
       <c r="D158" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2463,7 +2586,7 @@
         <v>158</v>
       </c>
       <c r="D160" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2484,13 +2607,16 @@
       <c r="C162" t="s">
         <v>167</v>
       </c>
+      <c r="D162" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>161</v>
       </c>
       <c r="D163" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2500,6 +2626,9 @@
       <c r="B164" t="s">
         <v>167</v>
       </c>
+      <c r="D164" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
@@ -2507,6 +2636,9 @@
       </c>
       <c r="C165" t="s">
         <v>167</v>
+      </c>
+      <c r="D165" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed merge between new SWC and SH, hopefully breaking as little as possible
</commit_message>
<xml_diff>
--- a/tools/merge.xlsx
+++ b/tools/merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="177">
   <si>
     <t>bullet.cpp</t>
   </si>
@@ -539,6 +539,12 @@
   </si>
   <si>
     <t>unneeded</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>* denotes file requiring later attention</t>
   </si>
 </sst>
 </file>
@@ -580,7 +586,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="4">
     <dxf>
       <font>
         <condense val="0"/>
@@ -614,78 +620,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -993,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1037,12 +971,15 @@
       <c r="C2" t="s">
         <v>167</v>
       </c>
+      <c r="D2" t="s">
+        <v>172</v>
+      </c>
       <c r="F2" t="s">
         <v>171</v>
       </c>
       <c r="G2">
         <f>COUNTIFS(D2:D165,"merged")+COUNTIFS(D2:D165,"unneeded")</f>
-        <v>116</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1055,12 +992,15 @@
       <c r="C3" t="s">
         <v>167</v>
       </c>
+      <c r="D3" t="s">
+        <v>172</v>
+      </c>
       <c r="F3" t="s">
         <v>173</v>
       </c>
       <c r="G3">
         <f>G2*100/G1</f>
-        <v>70.731707317073173</v>
+        <v>98.780487804878049</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1073,6 +1013,9 @@
       <c r="C4" t="s">
         <v>167</v>
       </c>
+      <c r="D4" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
@@ -1081,6 +1024,9 @@
       <c r="D5" t="s">
         <v>174</v>
       </c>
+      <c r="F5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
@@ -1152,6 +1098,9 @@
       <c r="C12" t="s">
         <v>167</v>
       </c>
+      <c r="D12" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
@@ -1209,6 +1158,9 @@
       <c r="C18" t="s">
         <v>167</v>
       </c>
+      <c r="D18" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
@@ -1247,6 +1199,9 @@
       <c r="C22" t="s">
         <v>167</v>
       </c>
+      <c r="D22" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
@@ -1266,6 +1221,9 @@
       <c r="C24" t="s">
         <v>167</v>
       </c>
+      <c r="D24" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
@@ -1323,6 +1281,9 @@
       <c r="C30" t="s">
         <v>167</v>
       </c>
+      <c r="D30" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
@@ -1345,8 +1306,11 @@
       <c r="C32" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="D32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1357,7 +1321,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1367,8 +1331,14 @@
       <c r="C34" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="D34" t="s">
+        <v>172</v>
+      </c>
+      <c r="E34" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1378,8 +1348,14 @@
       <c r="C35" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="D35" t="s">
+        <v>172</v>
+      </c>
+      <c r="E35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1390,7 +1366,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1401,7 +1377,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1411,8 +1387,14 @@
       <c r="C38" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="D38" t="s">
+        <v>172</v>
+      </c>
+      <c r="E38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1423,7 +1405,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1433,8 +1415,11 @@
       <c r="C40" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="D40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1442,7 +1427,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1452,8 +1437,14 @@
       <c r="C42" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="D42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1463,16 +1454,22 @@
       <c r="C43" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="D43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="C44" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="D44" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1480,7 +1477,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1490,8 +1487,11 @@
       <c r="C46" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="D46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1618,8 +1618,14 @@
       <c r="C59" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="D59" t="s">
+        <v>172</v>
+      </c>
+      <c r="E59" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1627,7 +1633,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1637,8 +1643,11 @@
       <c r="C61" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="D61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1646,7 +1655,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1654,7 +1663,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1662,7 +1671,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1670,7 +1679,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1678,7 +1687,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1688,8 +1697,11 @@
       <c r="C67" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="D67" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1699,8 +1711,11 @@
       <c r="C68" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="D68" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1710,8 +1725,11 @@
       <c r="C69" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="D69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1719,7 +1737,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1727,7 +1745,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1738,7 +1756,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1749,7 +1767,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1760,7 +1778,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -1768,7 +1786,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1778,8 +1796,11 @@
       <c r="C76" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -1789,8 +1810,11 @@
       <c r="C77" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -1800,8 +1824,14 @@
       <c r="C78" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="D78" t="s">
+        <v>172</v>
+      </c>
+      <c r="E78" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -1811,8 +1841,11 @@
       <c r="C79" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="D79" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -1823,7 +1856,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -1834,7 +1867,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -1845,7 +1878,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -1856,7 +1889,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -1867,7 +1900,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -1875,7 +1908,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -1886,7 +1919,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -1896,8 +1929,14 @@
       <c r="C87" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="D87" t="s">
+        <v>172</v>
+      </c>
+      <c r="E87" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -1907,8 +1946,14 @@
       <c r="C88" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="D88" t="s">
+        <v>172</v>
+      </c>
+      <c r="E88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -1919,7 +1964,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -1930,7 +1975,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -1941,7 +1986,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -1951,8 +1996,11 @@
       <c r="C92" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="D92" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -1960,7 +2008,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -1970,8 +2018,11 @@
       <c r="C94" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="D94" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -1979,7 +2030,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -1989,8 +2040,11 @@
       <c r="C96" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="D96" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -2000,8 +2054,11 @@
       <c r="C97" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="D97" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -2011,8 +2068,11 @@
       <c r="C98" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="D98" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -2023,7 +2083,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -2033,8 +2093,14 @@
       <c r="C100" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="D100" t="s">
+        <v>172</v>
+      </c>
+      <c r="E100" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -2044,16 +2110,25 @@
       <c r="C101" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="D101" t="s">
+        <v>172</v>
+      </c>
+      <c r="E101" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>100</v>
       </c>
       <c r="C102" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="D102" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -2061,7 +2136,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -2071,8 +2146,11 @@
       <c r="C104" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="D104" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -2080,7 +2158,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -2091,7 +2169,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -2102,7 +2180,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -2112,8 +2190,11 @@
       <c r="C108" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="D108" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -2121,7 +2202,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -2129,7 +2210,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -2137,7 +2218,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -2146,6 +2227,9 @@
       </c>
       <c r="C112" t="s">
         <v>167</v>
+      </c>
+      <c r="D112" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2166,6 +2250,9 @@
       <c r="C114" t="s">
         <v>167</v>
       </c>
+      <c r="D114" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
@@ -2245,6 +2332,9 @@
       <c r="C122" t="s">
         <v>167</v>
       </c>
+      <c r="D122" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
@@ -2256,6 +2346,9 @@
       <c r="C123" t="s">
         <v>167</v>
       </c>
+      <c r="D123" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
@@ -2267,6 +2360,9 @@
       <c r="C124" t="s">
         <v>167</v>
       </c>
+      <c r="D124" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
@@ -2373,6 +2469,9 @@
       <c r="C135" t="s">
         <v>167</v>
       </c>
+      <c r="D135" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
@@ -2384,6 +2483,9 @@
       <c r="C136" t="s">
         <v>167</v>
       </c>
+      <c r="D136" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
@@ -2395,6 +2497,9 @@
       <c r="C137" t="s">
         <v>167</v>
       </c>
+      <c r="D137" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
@@ -2580,6 +2685,9 @@
       <c r="C159" t="s">
         <v>167</v>
       </c>
+      <c r="D159" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
@@ -2599,6 +2707,9 @@
       <c r="C161" t="s">
         <v>167</v>
       </c>
+      <c r="D161" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
@@ -2643,10 +2754,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:C165">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"unique"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed compilation issues, the game compiles and runs now!
</commit_message>
<xml_diff>
--- a/tools/merge.xlsx
+++ b/tools/merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="177">
   <si>
     <t>bullet.cpp</t>
   </si>
@@ -927,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -979,7 +979,7 @@
       </c>
       <c r="G2">
         <f>COUNTIFS(D2:D165,"merged")+COUNTIFS(D2:D165,"unneeded")</f>
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="G3">
         <f>G2*100/G1</f>
-        <v>98.780487804878049</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1796,6 +1796,9 @@
       <c r="C76" t="s">
         <v>167</v>
       </c>
+      <c r="D76" t="s">
+        <v>172</v>
+      </c>
       <c r="E76" t="s">
         <v>175</v>
       </c>
@@ -1809,6 +1812,9 @@
       </c>
       <c r="C77" t="s">
         <v>167</v>
+      </c>
+      <c r="D77" t="s">
+        <v>172</v>
       </c>
       <c r="E77" t="s">
         <v>175</v>

</xml_diff>